<commit_message>
fixed chartEx multi copy bug
</commit_message>
<xml_diff>
--- a/tests/copyFromOneToManySheets/source.xlsx
+++ b/tests/copyFromOneToManySheets/source.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B532C86E-2AE6-4A25-ADD7-AA6A8D7DD279}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3223739B-7E30-4F99-A977-A8E1A7B0E914}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,11 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">earningsWorksheet1!$B$2:$B$16</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">earningsWorksheet1!$B$2:$B$22</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">earningsWorksheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">earningsWorksheet1!$C$2:$C$16</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">earningsWorksheet1!$C$2:$C$22</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">earningsWorksheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">earningsWorksheet1!$C$2:$C$16</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">earningsWorksheet1!$B$2:$B$6</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">earningsWorksheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">earningsWorksheet1!$C$2:$C$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3636,7 +3637,7 @@
         <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3674,10 +3675,84 @@
         <cx:series layoutId="waterfall" uniqueId="{66A7DFB8-8531-46BE-907C-E8CF04F4366D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>Ebit Per Share</cx:v>
             </cx:txData>
           </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:subtotals/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0.5"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>tester</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>tester</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="waterfall" uniqueId="{BBB8B932-6CC2-4CA8-88D3-5DBE963A6589}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:v>Ebit Per Share</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataLabels pos="outEnd">
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:subtotals/>
@@ -3859,6 +3934,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -5891,20 +6006,528 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="395">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>17391</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>117199</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>215348</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1243</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>124240</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>149087</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>472109</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>91109</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5933,16 +6556,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>10352</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>505238</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>157369</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>124239</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>91107</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>140803</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>24848</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5971,16 +6594,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>165651</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>57978</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>307350</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>41679</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>282502</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>49962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6009,16 +6632,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>207066</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>107674</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>231912</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57977</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>488674</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>165652</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>74543</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>16564</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -6054,8 +6677,86 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7636566" y="2774674"/>
-              <a:ext cx="4548808" cy="2724978"/>
+              <a:off x="5855803" y="1962977"/>
+              <a:ext cx="2294283" cy="1863587"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66260</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>173933</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>150745</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="8" name="Chart 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3DA2F89-A5D6-435F-BC76-FA68B76213CA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2625586" y="3702327"/>
+              <a:ext cx="2559325" cy="1591918"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6351,10 +7052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6528,6 +7229,7 @@
         <v>0.59089999999999998</v>
       </c>
     </row>
+    <row r="19" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0"/>
@@ -6540,7 +7242,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="B1" sqref="B1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6730,8 +7432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J39" sqref="J38:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8252,7 +8954,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>